<commit_message>
Battery Shield Support Stuff for AQS
Assembly diagram, stencil, BOM
</commit_message>
<xml_diff>
--- a/Battery Shield/battery-shield-smallinductor/Bill of Materials/bshield-bom-v1-131006.xlsx
+++ b/Battery Shield/battery-shield-smallinductor/Bill of Materials/bshield-bom-v1-131006.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -632,6 +632,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1481,8 +1482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1523,7 +1524,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="8">
         <f ca="1">TODAY()</f>
-        <v>41554</v>
+        <v>41653</v>
       </c>
     </row>
     <row r="4" spans="2:11">
@@ -2110,7 +2111,7 @@
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="53" t="s">
         <v>128</v>
@@ -2358,7 +2359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>